<commit_message>
Corrected the population and the GTP of Slovenia to csv and excel
</commit_message>
<xml_diff>
--- a/Budget_Surfers/src/main/resourses/Gdp_population_euz.xlsx
+++ b/Budget_Surfers/src/main/resourses/Gdp_population_euz.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsta1\Budget\Budget_Surfers\src\main\resourses\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eugen\Budget\Budget_Surfers\src\main\resourses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D070F55C-9AFA-4A04-A045-CA53DC2BE1DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0292DA-E0E3-480E-8C11-6E399B94DB62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{44CB0367-DF64-4552-A937-215DCECEADD0}"/>
   </bookViews>
@@ -192,7 +192,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -208,7 +208,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Θέμα του Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -527,7 +527,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -756,10 +756,10 @@
       </c>
       <c r="B19" s="6">
         <f xml:space="preserve"> 34400 * C19</f>
-        <v>7703845600</v>
+        <v>77038456000</v>
       </c>
       <c r="C19" s="5">
-        <v>223949</v>
+        <v>2239490</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>